<commit_message>
code and file updates
</commit_message>
<xml_diff>
--- a/Data Samples/Death_records_data_sample.xlsx
+++ b/Data Samples/Death_records_data_sample.xlsx
@@ -14039,8 +14039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -71637,6 +71637,6 @@
     <hyperlink ref="A1952" r:id="rId1" display="HEALTH PERMIT DATA"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>